<commit_message>
Added warning message for missing countries in aggregates, added inflation adjustment for GNI per capita and epsilon calculation, added gdp deflator forecasts for value transfers into the futuree
</commit_message>
<xml_diff>
--- a/data-raw/income_class.xlsx
+++ b/data-raw/income_class.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/mela_rse-web_it/Documents/R/miei_pacchetti/btransfer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14B52E61-D1A9-4524-A7D9-5A6C65FDF2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{14B52E61-D1A9-4524-A7D9-5A6C65FDF2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB5C75EB-0F5B-4E7A-AE79-8506EDCD1760}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="income_class" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -609,9 +609,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -649,7 +649,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -755,7 +755,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -897,18 +897,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,13 +944,13 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1045</v>
+        <v>1135</v>
       </c>
       <c r="E2">
         <v>1.2</v>
       </c>
       <c r="F2">
-        <v>2021</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -961,16 +961,16 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>1046</v>
+        <v>1136</v>
       </c>
       <c r="D3">
-        <v>4095</v>
+        <v>4495</v>
       </c>
       <c r="E3">
         <v>0.8</v>
       </c>
       <c r="F3">
-        <v>2021</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -981,16 +981,16 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>4096</v>
+        <v>4496</v>
       </c>
       <c r="D4">
-        <v>12695</v>
+        <v>13935</v>
       </c>
       <c r="E4">
         <v>0.5</v>
       </c>
       <c r="F4">
-        <v>2021</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1001,7 +1001,7 @@
         <v>13</v>
       </c>
       <c r="C5">
-        <v>12696</v>
+        <v>13936</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -1010,7 +1010,7 @@
         <v>0.2</v>
       </c>
       <c r="F5">
-        <v>2021</v>
+        <v>2024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
World bank country classification FY 2023, latest compatible with other macroeconomic variables
</commit_message>
<xml_diff>
--- a/data-raw/income_class.xlsx
+++ b/data-raw/income_class.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/mela_rse-web_it/Documents/R/miei_pacchetti/btransfer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{14B52E61-D1A9-4524-A7D9-5A6C65FDF2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB5C75EB-0F5B-4E7A-AE79-8506EDCD1760}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{14B52E61-D1A9-4524-A7D9-5A6C65FDF2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED654B42-BCE4-472C-A95A-3F1CF22FE4D6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +202,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -548,8 +556,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -606,6 +615,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -908,7 +921,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F3" sqref="F3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,7 +963,7 @@
         <v>1.2</v>
       </c>
       <c r="F2">
-        <v>2024</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -964,13 +977,13 @@
         <v>1136</v>
       </c>
       <c r="D3">
-        <v>4495</v>
+        <v>4465</v>
       </c>
       <c r="E3">
         <v>0.8</v>
       </c>
-      <c r="F3">
-        <v>2024</v>
+      <c r="F3" s="1">
+        <v>2023</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -981,16 +994,16 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>4496</v>
+        <v>4466</v>
       </c>
       <c r="D4">
-        <v>13935</v>
+        <v>13845</v>
       </c>
       <c r="E4">
         <v>0.5</v>
       </c>
-      <c r="F4">
-        <v>2024</v>
+      <c r="F4" s="1">
+        <v>2023</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1001,7 +1014,7 @@
         <v>13</v>
       </c>
       <c r="C5">
-        <v>13936</v>
+        <v>13846</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -1009,8 +1022,8 @@
       <c r="E5">
         <v>0.2</v>
       </c>
-      <c r="F5">
-        <v>2024</v>
+      <c r="F5" s="1">
+        <v>2023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>